<commit_message>
update after website test
</commit_message>
<xml_diff>
--- a/Experiment3/Text_stimuli_exp3.xlsx
+++ b/Experiment3/Text_stimuli_exp3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\SPR_online\Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECCD4BA-4F37-4F9C-8274-DB4B9B5A328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB24B50-5A1D-48C5-911B-E943C1E2E265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -255,13 +255,13 @@
     <t>According to the passage, time was measured with sundials only for a couple of decades because a better method was soon discovered.</t>
   </si>
   <si>
-    <t xml:space="preserve">According to the passage, cities would not always be aligned in the time they use. </t>
-  </si>
-  <si>
     <t>According to the passage, steam sterilization has unlimited uses in the treatment of medical waste.</t>
   </si>
   <si>
     <t>According to the passage, plastic bottles take 15 years to disintegrate.</t>
+  </si>
+  <si>
+    <t>According to the passage, cities would not always use exactly the same time.</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1105,7 @@
         <v>59</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
@@ -1186,7 +1186,7 @@
         <v>66</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G21" s="12">
         <v>1</v>

</xml_diff>

<commit_message>
some changes in preproc
</commit_message>
<xml_diff>
--- a/Experiment3/Text_stimuli_exp3.xlsx
+++ b/Experiment3/Text_stimuli_exp3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\SPR_online\Experiment3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB24B50-5A1D-48C5-911B-E943C1E2E265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105EFA10-2048-4E05-AD41-2F42FF087248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,7 +647,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,8 +1291,8 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H26" s="2">
-        <f>SUM(H2:H16)</f>
-        <v>801</v>
+        <f>SUM(H2:H21)</f>
+        <v>1049</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>